<commit_message>
Updated CHE model - 2025-08-09 23:29
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_CHE/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78583848-7465-4B77-BBD4-DADD8B9819B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C971D5-3E81-4812-ABAE-BDF139DD8049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -540,21 +540,21 @@
     <t>com_fr</t>
   </si>
   <si>
+    <t>process</t>
+  </si>
+  <si>
     <t>commodity</t>
   </si>
   <si>
-    <t>process</t>
-  </si>
-  <si>
     <t>S1aH1</t>
   </si>
   <si>
+    <t>IMPNRGZ</t>
+  </si>
+  <si>
     <t>elc_sol-CHE</t>
   </si>
   <si>
-    <t>IMPNRGZ</t>
-  </si>
-  <si>
     <t>S1aH2</t>
   </si>
   <si>
@@ -903,10 +903,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S2b0205h09,S3aH2,S3d0419h16,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4,S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S3d0419h10,S3d0419h13,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6,S3c0312h08,S3d0419h08,S4aH2,S3aH3,S3c0312h10,S3c0312h07,S4aH5,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S2b0205h10,S2b0205h18,S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S3c0312h18,S3d0419h09</t>
-  </si>
-  <si>
-    <t>S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S3aH8,S3c0312h05,S3d0419h24,S2b0205h02,S3c0312h06,S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S2b0205h22,S3aH1,S3c0312h24,S1aH8,S3c0312h19,S5aH1,S2b0205h03,S3d0419h03,S2aH1,S2b0205h21,S3aH7,S5aH8,S3d0419h02,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23,S3c0312h01,S3c0312h23,S3d0419h21,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S2b0205h04,S3d0419h20,S4aH8,S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2aH8,S3d0419h01</t>
+    <t>S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S2b0205h10,S2b0205h18,S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S3c0312h18,S3d0419h09,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4,S2b0205h09,S3aH2,S3d0419h16,S3aH3,S3c0312h10,S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S3d0419h10,S3d0419h13,S3c0312h07,S4aH5,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S3c0312h08,S3d0419h08,S4aH2,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6</t>
+  </si>
+  <si>
+    <t>S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2b0205h04,S3d0419h20,S4aH8,S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S2aH8,S3d0419h01,S3aH8,S3c0312h05,S3d0419h24,S3d0419h02,S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S2b0205h22,S3aH1,S3c0312h24,S3c0312h01,S3c0312h23,S3d0419h21,S1aH8,S3c0312h19,S5aH1,S2aH1,S2b0205h21,S3aH7,S5aH8,S2b0205h02,S3c0312h06,S2b0205h03,S3d0419h03,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S3aH8,S3c0312h05,S3d0419h24,S2b0205h02,S3c0312h06,S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S2b0205h22,S3aH1,S3c0312h24,S1aH8,S3c0312h19,S5aH1,S2b0205h03,S3d0419h03,S2aH1,S2b0205h21,S3aH7,S5aH8,S3d0419h02,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23,S3c0312h01,S3c0312h23,S3d0419h21,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S2b0205h04,S3d0419h20,S4aH8,S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2aH8,S3d0419h01</v>
+        <v>S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2b0205h04,S3d0419h20,S4aH8,S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S2aH8,S3d0419h01,S3aH8,S3c0312h05,S3d0419h24,S3d0419h02,S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S2b0205h22,S3aH1,S3c0312h24,S3c0312h01,S3c0312h23,S3d0419h21,S1aH8,S3c0312h19,S5aH1,S2aH1,S2b0205h21,S3aH7,S5aH8,S2b0205h02,S3c0312h06,S2b0205h03,S3d0419h03,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S2b0205h09,S3aH2,S3d0419h16,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4,S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S3d0419h10,S3d0419h13,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6,S3c0312h08,S3d0419h08,S4aH2,S3aH3,S3c0312h10,S3c0312h07,S4aH5,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S2b0205h10,S2b0205h18,S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S3c0312h18,S3d0419h09</v>
+        <v>S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S2b0205h10,S2b0205h18,S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S3c0312h18,S3d0419h09,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4,S2b0205h09,S3aH2,S3d0419h16,S3aH3,S3c0312h10,S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S3d0419h10,S3d0419h13,S3c0312h07,S4aH5,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S3c0312h08,S3d0419h08,S4aH2,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2122,7 +2122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14E42F3-1507-4DD9-A4BB-A96E2F38CD4B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAFD2E5-38D4-4ACF-8806-F80A74A520C0}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2836,7 +2836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3198E8A6-B26B-4874-BC0F-E359AFD33405}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB4873C-3394-410D-9551-F4CF5F7FA939}">
   <dimension ref="B2:O115"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2909,16 +2909,16 @@
         <v>5.7499999999999999E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K4" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
       <c r="M4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="N4">
-        <v>7.9527811637903387E-2</v>
+        <v>9.7812279463655616E-2</v>
       </c>
       <c r="O4" t="s">
         <v>294</v>
@@ -2944,10 +2944,10 @@
         <v>9.2299999999999999E-4</v>
       </c>
       <c r="J5" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K5" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
       <c r="M5" t="s">
         <v>80</v>
@@ -2979,16 +2979,16 @@
         <v>1.0119999999999999E-3</v>
       </c>
       <c r="J6" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K6" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N6">
-        <v>0.86333483030730718</v>
+        <v>8.0605632899210883E-2</v>
       </c>
       <c r="O6" t="s">
         <v>294</v>
@@ -3014,16 +3014,16 @@
         <v>1.0999999999999998E-3</v>
       </c>
       <c r="J7" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K7" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
       <c r="M7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N7">
-        <v>8.0605632899210883E-2</v>
+        <v>0.86333483030730718</v>
       </c>
       <c r="O7" t="s">
         <v>294</v>
@@ -3049,16 +3049,16 @@
         <v>8.9529999999999992E-3</v>
       </c>
       <c r="J8" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K8" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
       <c r="M8" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="N8">
-        <v>9.7812279463655616E-2</v>
+        <v>7.9527811637903387E-2</v>
       </c>
       <c r="O8" t="s">
         <v>294</v>
@@ -3084,10 +3084,10 @@
         <v>3.2410000000000001E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K9" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.45">
@@ -3110,10 +3110,10 @@
         <v>9.4909999999999994E-3</v>
       </c>
       <c r="J10" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K10" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.45">
@@ -3136,10 +3136,10 @@
         <v>3.1855000000000001E-2</v>
       </c>
       <c r="J11" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K11" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.45">
@@ -3162,10 +3162,10 @@
         <v>1.5494000000000001E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K12" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.45">
@@ -3188,10 +3188,10 @@
         <v>1.4910000000000001E-3</v>
       </c>
       <c r="J13" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K13" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.45">
@@ -3214,10 +3214,10 @@
         <v>2.0230000000000001E-3</v>
       </c>
       <c r="J14" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K14" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.45">
@@ -3240,10 +3240,10 @@
         <v>2.4069999999999999E-3</v>
       </c>
       <c r="J15" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K15" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.45">
@@ -3266,10 +3266,10 @@
         <v>1.6163E-2</v>
       </c>
       <c r="J16" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K16" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.45">
@@ -3292,10 +3292,10 @@
         <v>1.6781000000000001E-2</v>
       </c>
       <c r="J17" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K17" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.45">
@@ -3318,10 +3318,10 @@
         <v>6.2459999999999998E-3</v>
       </c>
       <c r="J18" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K18" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.45">
@@ -3344,10 +3344,10 @@
         <v>1.2119E-2</v>
       </c>
       <c r="J19" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K19" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.45">
@@ -3370,10 +3370,10 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K20" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.45">
@@ -3396,10 +3396,10 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K21" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.45">
@@ -3422,10 +3422,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K22" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.45">
@@ -3448,10 +3448,10 @@
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="J23" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K23" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.45">
@@ -3474,10 +3474,10 @@
         <v>2.8400000000000002E-4</v>
       </c>
       <c r="J24" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K24" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.45">
@@ -3500,10 +3500,10 @@
         <v>4.6099999999999998E-4</v>
       </c>
       <c r="J25" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K25" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.45">
@@ -3526,10 +3526,10 @@
         <v>7.2800000000000002E-4</v>
       </c>
       <c r="J26" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K26" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.45">
@@ -3552,10 +3552,10 @@
         <v>1.17E-3</v>
       </c>
       <c r="J27" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K27" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.45">
@@ -3578,10 +3578,10 @@
         <v>3.3010000000000001E-3</v>
       </c>
       <c r="J28" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K28" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.45">
@@ -3604,10 +3604,10 @@
         <v>7.4070000000000004E-3</v>
       </c>
       <c r="J29" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K29" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.45">
@@ -3630,10 +3630,10 @@
         <v>8.4729999999999996E-3</v>
       </c>
       <c r="J30" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K30" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.45">
@@ -3656,10 +3656,10 @@
         <v>7.4070000000000004E-3</v>
       </c>
       <c r="J31" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K31" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.45">
@@ -3682,10 +3682,10 @@
         <v>1.1738999999999999E-2</v>
       </c>
       <c r="J32" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K32" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.45">
@@ -3708,10 +3708,10 @@
         <v>9.4619999999999999E-3</v>
       </c>
       <c r="J33" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K33" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.45">
@@ -3734,10 +3734,10 @@
         <v>1.6534E-2</v>
       </c>
       <c r="J34" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K34" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.45">
@@ -3760,10 +3760,10 @@
         <v>9.0060000000000001E-3</v>
       </c>
       <c r="J35" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K35" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.45">
@@ -3786,10 +3786,10 @@
         <v>3.6120000000000002E-3</v>
       </c>
       <c r="J36" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K36" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.45">
@@ -3812,10 +3812,10 @@
         <v>2.0579999999999999E-3</v>
       </c>
       <c r="J37" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K37" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.45">
@@ -3838,10 +3838,10 @@
         <v>5.5000000000000003E-4</v>
       </c>
       <c r="J38" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K38" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.45">
@@ -3864,10 +3864,10 @@
         <v>2.8400000000000002E-4</v>
       </c>
       <c r="J39" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K39" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.45">
@@ -3890,10 +3890,10 @@
         <v>1.1900000000000001E-4</v>
       </c>
       <c r="J40" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K40" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.45">
@@ -3916,10 +3916,10 @@
         <v>1.95E-4</v>
       </c>
       <c r="J41" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K41" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.45">
@@ -3942,10 +3942,10 @@
         <v>8.1700000000000002E-4</v>
       </c>
       <c r="J42" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K42" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.45">
@@ -3968,10 +3968,10 @@
         <v>1.17E-3</v>
       </c>
       <c r="J43" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K43" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.45">
@@ -3994,10 +3994,10 @@
         <v>6.0167999999999999E-2</v>
       </c>
       <c r="J44" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K44" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.45">
@@ -4020,10 +4020,10 @@
         <v>6.483E-3</v>
       </c>
       <c r="J45" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K45" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.45">
@@ -4046,10 +4046,10 @@
         <v>1.0378E-2</v>
       </c>
       <c r="J46" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K46" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.45">
@@ -4072,10 +4072,10 @@
         <v>2.5076000000000001E-2</v>
       </c>
       <c r="J47" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K47" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.45">
@@ -4098,10 +4098,10 @@
         <v>0.163051</v>
       </c>
       <c r="J48" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K48" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.45">
@@ -4124,10 +4124,10 @@
         <v>0.20358999999999999</v>
       </c>
       <c r="J49" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K49" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.45">
@@ -4150,10 +4150,10 @@
         <v>2.3820000000000001E-2</v>
       </c>
       <c r="J50" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K50" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.45">
@@ -4176,10 +4176,10 @@
         <v>2.8472000000000001E-2</v>
       </c>
       <c r="J51" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K51" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.45">
@@ -4202,10 +4202,10 @@
         <v>0</v>
       </c>
       <c r="J52" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K52" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.45">
@@ -4228,10 +4228,10 @@
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K53" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.45">
@@ -4254,10 +4254,10 @@
         <v>0</v>
       </c>
       <c r="J54" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K54" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.45">
@@ -4280,10 +4280,10 @@
         <v>0</v>
       </c>
       <c r="J55" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K55" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.45">
@@ -4306,10 +4306,10 @@
         <v>0</v>
       </c>
       <c r="J56" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K56" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.45">
@@ -4332,10 +4332,10 @@
         <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K57" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.45">
@@ -4358,10 +4358,10 @@
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K58" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.45">
@@ -4384,10 +4384,10 @@
         <v>0</v>
       </c>
       <c r="J59" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K59" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.45">
@@ -4410,10 +4410,10 @@
         <v>0</v>
       </c>
       <c r="J60" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K60" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.45">
@@ -4436,10 +4436,10 @@
         <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K61" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.45">
@@ -4462,10 +4462,10 @@
         <v>0</v>
       </c>
       <c r="J62" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K62" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.45">
@@ -4488,10 +4488,10 @@
         <v>0</v>
       </c>
       <c r="J63" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K63" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.45">
@@ -4514,10 +4514,10 @@
         <v>0</v>
       </c>
       <c r="J64" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K64" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.45">
@@ -4540,10 +4540,10 @@
         <v>0</v>
       </c>
       <c r="J65" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K65" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.45">
@@ -4566,10 +4566,10 @@
         <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K66" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.45">
@@ -4592,10 +4592,10 @@
         <v>3.7300000000000001E-4</v>
       </c>
       <c r="J67" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K67" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.45">
@@ -4618,10 +4618,10 @@
         <v>1.17E-3</v>
       </c>
       <c r="J68" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K68" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.45">
@@ -4644,10 +4644,10 @@
         <v>1.436E-3</v>
       </c>
       <c r="J69" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K69" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.45">
@@ -4670,10 +4670,10 @@
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K70" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.45">
@@ -4696,10 +4696,10 @@
         <v>0</v>
       </c>
       <c r="J71" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K71" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.45">
@@ -4722,10 +4722,10 @@
         <v>0</v>
       </c>
       <c r="J72" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K72" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.45">
@@ -4748,10 +4748,10 @@
         <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K73" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.45">
@@ -4774,10 +4774,10 @@
         <v>0</v>
       </c>
       <c r="J74" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K74" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.45">
@@ -4800,10 +4800,10 @@
         <v>0</v>
       </c>
       <c r="J75" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K75" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.45">
@@ -4826,10 +4826,10 @@
         <v>0</v>
       </c>
       <c r="J76" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K76" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.45">
@@ -4852,10 +4852,10 @@
         <v>0</v>
       </c>
       <c r="J77" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K77" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.45">
@@ -4878,10 +4878,10 @@
         <v>0</v>
       </c>
       <c r="J78" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K78" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.45">
@@ -4904,10 +4904,10 @@
         <v>0</v>
       </c>
       <c r="J79" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K79" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.45">
@@ -4930,10 +4930,10 @@
         <v>0</v>
       </c>
       <c r="J80" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K80" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.45">
@@ -4956,10 +4956,10 @@
         <v>0</v>
       </c>
       <c r="J81" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K81" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.45">
@@ -4982,10 +4982,10 @@
         <v>0</v>
       </c>
       <c r="J82" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K82" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.45">
@@ -5008,10 +5008,10 @@
         <v>0</v>
       </c>
       <c r="J83" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K83" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.45">
@@ -5034,10 +5034,10 @@
         <v>0</v>
       </c>
       <c r="J84" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K84" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.45">
@@ -5060,10 +5060,10 @@
         <v>0</v>
       </c>
       <c r="J85" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K85" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.45">
@@ -5086,10 +5086,10 @@
         <v>0</v>
       </c>
       <c r="J86" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K86" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.45">
@@ -5112,10 +5112,10 @@
         <v>0</v>
       </c>
       <c r="J87" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K87" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.45">
@@ -5138,10 +5138,10 @@
         <v>0</v>
       </c>
       <c r="J88" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K88" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.45">
@@ -5164,10 +5164,10 @@
         <v>0</v>
       </c>
       <c r="J89" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K89" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.45">
@@ -5190,10 +5190,10 @@
         <v>0</v>
       </c>
       <c r="J90" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K90" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.45">
@@ -5216,10 +5216,10 @@
         <v>0</v>
       </c>
       <c r="J91" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K91" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.45">
@@ -5242,10 +5242,10 @@
         <v>0</v>
       </c>
       <c r="J92" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K92" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.45">
@@ -5268,10 +5268,10 @@
         <v>0</v>
       </c>
       <c r="J93" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K93" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.45">
@@ -5294,10 +5294,10 @@
         <v>0</v>
       </c>
       <c r="J94" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K94" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.45">
@@ -5320,10 +5320,10 @@
         <v>0</v>
       </c>
       <c r="J95" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K95" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.45">
@@ -5346,10 +5346,10 @@
         <v>0</v>
       </c>
       <c r="J96" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K96" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.45">
@@ -5372,10 +5372,10 @@
         <v>0</v>
       </c>
       <c r="J97" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K97" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.45">
@@ -5398,10 +5398,10 @@
         <v>0</v>
       </c>
       <c r="J98" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K98" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.45">
@@ -5424,10 +5424,10 @@
         <v>0</v>
       </c>
       <c r="J99" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K99" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.45">
@@ -5450,10 +5450,10 @@
         <v>1.9053E-2</v>
       </c>
       <c r="J100" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K100" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.45">
@@ -5476,10 +5476,10 @@
         <v>3.431E-3</v>
       </c>
       <c r="J101" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K101" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.45">
@@ -5502,10 +5502,10 @@
         <v>1.4496999999999999E-2</v>
       </c>
       <c r="J102" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K102" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.45">
@@ -5528,10 +5528,10 @@
         <v>2.8079E-2</v>
       </c>
       <c r="J103" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K103" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.45">
@@ -5554,10 +5554,10 @@
         <v>0.10306800000000001</v>
       </c>
       <c r="J104" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K104" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.45">
@@ -5580,10 +5580,10 @@
         <v>4.0084000000000002E-2</v>
       </c>
       <c r="J105" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K105" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.45">
@@ -5606,10 +5606,10 @@
         <v>2.2720000000000001E-3</v>
       </c>
       <c r="J106" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K106" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.45">
@@ -5632,10 +5632,10 @@
         <v>1.0816000000000001E-2</v>
       </c>
       <c r="J107" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K107" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.45">
@@ -5658,10 +5658,10 @@
         <v>2.5250000000000003E-3</v>
       </c>
       <c r="J108" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K108" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.45">
@@ -5684,10 +5684,10 @@
         <v>0</v>
       </c>
       <c r="J109" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K109" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.45">
@@ -5710,10 +5710,10 @@
         <v>0</v>
       </c>
       <c r="J110" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K110" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.45">
@@ -5736,10 +5736,10 @@
         <v>0</v>
       </c>
       <c r="J111" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K111" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.45">
@@ -5762,10 +5762,10 @@
         <v>6.87E-4</v>
       </c>
       <c r="J112" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K112" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.45">
@@ -5788,10 +5788,10 @@
         <v>1.774E-3</v>
       </c>
       <c r="J113" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K113" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.45">
@@ -5814,10 +5814,10 @@
         <v>1.1900000000000001E-4</v>
       </c>
       <c r="J114" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K114" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.45">
@@ -5840,10 +5840,10 @@
         <v>2.0900000000000001E-4</v>
       </c>
       <c r="J115" t="s">
-        <v>283</v>
+        <v>169</v>
       </c>
       <c r="K115" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -5852,7 +5852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EB931D-CF47-4285-BB99-966EF1FBC7FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A566AB-EEC3-4260-A8FA-B442FFEDD9FB}">
   <dimension ref="B2:O227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5881,10 +5881,10 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I3" t="s">
         <v>70</v>
@@ -5893,7 +5893,7 @@
         <v>165</v>
       </c>
       <c r="M3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N3" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-10 01:19
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_CHE/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C971D5-3E81-4812-ABAE-BDF139DD8049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89450AA9-5838-4E38-AA18-15589B806304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -903,10 +903,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S2b0205h10,S2b0205h18,S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S3c0312h18,S3d0419h09,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4,S2b0205h09,S3aH2,S3d0419h16,S3aH3,S3c0312h10,S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S3d0419h10,S3d0419h13,S3c0312h07,S4aH5,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S3c0312h08,S3d0419h08,S4aH2,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6</t>
-  </si>
-  <si>
-    <t>S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2b0205h04,S3d0419h20,S4aH8,S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S2aH8,S3d0419h01,S3aH8,S3c0312h05,S3d0419h24,S3d0419h02,S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S2b0205h22,S3aH1,S3c0312h24,S3c0312h01,S3c0312h23,S3d0419h21,S1aH8,S3c0312h19,S5aH1,S2aH1,S2b0205h21,S3aH7,S5aH8,S2b0205h02,S3c0312h06,S2b0205h03,S3d0419h03,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23</t>
+    <t>S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S2b0205h09,S3aH2,S3d0419h16,S3c0312h07,S4aH5,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S3c0312h18,S3d0419h09,S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S2b0205h10,S2b0205h18,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S3d0419h10,S3d0419h13,S3c0312h08,S3d0419h08,S4aH2,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6,S3aH3,S3c0312h10,S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4</t>
+  </si>
+  <si>
+    <t>S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S3aH8,S3c0312h05,S3d0419h24,S3c0312h01,S3c0312h23,S3d0419h21,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S1aH8,S3c0312h19,S5aH1,S2aH8,S3d0419h01,S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2b0205h04,S3d0419h20,S4aH8,S2b0205h02,S3c0312h06,S2b0205h22,S3aH1,S3c0312h24,S2aH1,S2b0205h21,S3aH7,S5aH8,S2b0205h03,S3d0419h03,S3d0419h02,S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2b0205h04,S3d0419h20,S4aH8,S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S2aH8,S3d0419h01,S3aH8,S3c0312h05,S3d0419h24,S3d0419h02,S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S2b0205h22,S3aH1,S3c0312h24,S3c0312h01,S3c0312h23,S3d0419h21,S1aH8,S3c0312h19,S5aH1,S2aH1,S2b0205h21,S3aH7,S5aH8,S2b0205h02,S3c0312h06,S2b0205h03,S3d0419h03,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23</v>
+        <v>S1aH7,S3c0312h03,S3c0312h22,S3d0419h19,S4aH7,S5aH7,S3aH8,S3c0312h05,S3d0419h24,S3c0312h01,S3c0312h23,S3d0419h21,S2b0205h05,S2b0205h19,S3c0312h04,S3c0312h20,S1aH8,S3c0312h19,S5aH1,S2aH8,S3d0419h01,S2b0205h20,S2b0205h24,S3d0419h04,S3d0419h05,S4aH1,S2b0205h04,S3d0419h20,S4aH8,S2b0205h02,S3c0312h06,S2b0205h22,S3aH1,S3c0312h24,S2aH1,S2b0205h21,S3aH7,S5aH8,S2b0205h03,S3d0419h03,S3d0419h02,S2b0205h01,S2b0205h06,S3d0419h06,S3d0419h22,S1aH1,S2aH7,S2b0205h23,S3c0312h02,S3c0312h21,S3d0419h23</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S2b0205h10,S2b0205h18,S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S3c0312h18,S3d0419h09,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4,S2b0205h09,S3aH2,S3d0419h16,S3aH3,S3c0312h10,S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S3d0419h10,S3d0419h13,S3c0312h07,S4aH5,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S3c0312h08,S3d0419h08,S4aH2,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6</v>
+        <v>S1aH3,S2b0205h13,S3c0312h12,S3d0419h17,S2b0205h09,S3aH2,S3d0419h16,S3c0312h07,S4aH5,S1aH5,S2aH4,S2aH5,S3c0312h16,S3d0419h12,S5aH2,S5aH5,S2aH6,S3aH5,S3c0312h13,S3c0312h17,S3d0419h07,S3d0419h14,S5aH3,S3c0312h18,S3d0419h09,S1aH4,S2aH2,S2b0205h11,S3c0312h09,S4aH6,S2b0205h10,S2b0205h18,S2b0205h14,S2b0205h15,S2b0205h17,S3c0312h11,S3d0419h11,S3d0419h15,S5aH4,S3d0419h10,S3d0419h13,S3c0312h08,S3d0419h08,S4aH2,S1aH2,S2aH3,S2b0205h12,S2b0205h16,S3aH6,S5aH6,S3aH3,S3c0312h10,S1aH6,S2b0205h07,S2b0205h08,S3c0312h15,S3aH4,S3c0312h14,S3d0419h18,S4aH3,S4aH4</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2122,7 +2122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAFD2E5-38D4-4ACF-8806-F80A74A520C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AD8F47-4E2A-433A-B66F-92F60AD9B5A9}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2836,7 +2836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB4873C-3394-410D-9551-F4CF5F7FA939}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF854AB-C3A7-4FB8-B206-481A78A04705}">
   <dimension ref="B2:O115"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2915,10 +2915,10 @@
         <v>283</v>
       </c>
       <c r="M4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N4">
-        <v>9.7812279463655616E-2</v>
+        <v>7.8719445691922768E-2</v>
       </c>
       <c r="O4" t="s">
         <v>294</v>
@@ -2950,10 +2950,10 @@
         <v>283</v>
       </c>
       <c r="M5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="N5">
-        <v>7.8719445691922754E-2</v>
+        <v>7.9527811637903401E-2</v>
       </c>
       <c r="O5" t="s">
         <v>294</v>
@@ -2985,10 +2985,10 @@
         <v>283</v>
       </c>
       <c r="M6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N6">
-        <v>8.0605632899210883E-2</v>
+        <v>0.8633348303073074</v>
       </c>
       <c r="O6" t="s">
         <v>294</v>
@@ -3020,10 +3020,10 @@
         <v>283</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N7">
-        <v>0.86333483030730718</v>
+        <v>8.0605632899210897E-2</v>
       </c>
       <c r="O7" t="s">
         <v>294</v>
@@ -3055,10 +3055,10 @@
         <v>283</v>
       </c>
       <c r="M8" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="N8">
-        <v>7.9527811637903387E-2</v>
+        <v>9.781227946365563E-2</v>
       </c>
       <c r="O8" t="s">
         <v>294</v>
@@ -5852,7 +5852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A566AB-EEC3-4260-A8FA-B442FFEDD9FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D789A4-4271-48EC-9A2E-7A8796F46464}">
   <dimension ref="B2:O227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
flo_fr instead of com_fr
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_CHE/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B587B1-4611-4E00-9F34-724A3B96FDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBE57F3-7E2D-4F8E-9A7F-5E7EBCE448B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="12682" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
   <sheets>
     <sheet name="ev_charging_uc" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="307">
   <si>
     <t>UC_N</t>
   </si>
@@ -955,6 +955,12 @@
   </si>
   <si>
     <t>~TFM_INS-AT</t>
+  </si>
+  <si>
+    <t>flo_fr</t>
+  </si>
+  <si>
+    <t>~TFM_DINS-AT: limtype=UP</t>
   </si>
 </sst>
 </file>
@@ -2869,16 +2875,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6138DF07-5FE9-46F6-804C-AEEFE72DE2EC}">
   <dimension ref="B2:O123"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>291</v>
       </c>
       <c r="H2" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="M2" t="s">
         <v>304</v>
@@ -2901,10 +2912,10 @@
         <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>166</v>
+        <v>305</v>
       </c>
       <c r="J3" t="s">
-        <v>167</v>
+        <v>302</v>
       </c>
       <c r="K3" t="s">
         <v>168</v>
@@ -2938,8 +2949,9 @@
       <c r="I4">
         <v>4.3693999999999997E-2</v>
       </c>
-      <c r="J4" t="s">
-        <v>170</v>
+      <c r="J4" t="str">
+        <f>K4</f>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K4" t="s">
         <v>292</v>
@@ -2973,8 +2985,9 @@
       <c r="I5">
         <v>6.0470000000000003E-3</v>
       </c>
-      <c r="J5" t="s">
-        <v>170</v>
+      <c r="J5" t="str">
+        <f t="shared" ref="J5:J68" si="0">K5</f>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K5" t="s">
         <v>292</v>
@@ -3008,8 +3021,9 @@
       <c r="I6">
         <v>6.0879999999999997E-3</v>
       </c>
-      <c r="J6" t="s">
-        <v>170</v>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K6" t="s">
         <v>292</v>
@@ -3043,8 +3057,9 @@
       <c r="I7">
         <v>6.2369999999999995E-3</v>
       </c>
-      <c r="J7" t="s">
-        <v>170</v>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K7" t="s">
         <v>292</v>
@@ -3078,8 +3093,9 @@
       <c r="I8">
         <v>3.3429E-2</v>
       </c>
-      <c r="J8" t="s">
-        <v>170</v>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K8" t="s">
         <v>292</v>
@@ -3113,8 +3129,9 @@
       <c r="I9">
         <v>7.358E-3</v>
       </c>
-      <c r="J9" t="s">
-        <v>170</v>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K9" t="s">
         <v>292</v>
@@ -3148,8 +3165,9 @@
       <c r="I10">
         <v>7.4980000000000003E-3</v>
       </c>
-      <c r="J10" t="s">
-        <v>170</v>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K10" t="s">
         <v>292</v>
@@ -3174,8 +3192,9 @@
       <c r="I11">
         <v>4.8984E-2</v>
       </c>
-      <c r="J11" t="s">
-        <v>170</v>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K11" t="s">
         <v>292</v>
@@ -3200,8 +3219,9 @@
       <c r="I12">
         <v>1.02E-4</v>
       </c>
-      <c r="J12" t="s">
-        <v>170</v>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K12" t="s">
         <v>292</v>
@@ -3226,8 +3246,9 @@
       <c r="I13">
         <v>1.02E-4</v>
       </c>
-      <c r="J13" t="s">
-        <v>170</v>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K13" t="s">
         <v>292</v>
@@ -3252,8 +3273,9 @@
       <c r="I14">
         <v>1.02E-4</v>
       </c>
-      <c r="J14" t="s">
-        <v>170</v>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K14" t="s">
         <v>292</v>
@@ -3278,8 +3300,9 @@
       <c r="I15">
         <v>1.06E-4</v>
       </c>
-      <c r="J15" t="s">
-        <v>170</v>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K15" t="s">
         <v>292</v>
@@ -3304,8 +3327,9 @@
       <c r="I16">
         <v>1.37E-4</v>
       </c>
-      <c r="J16" t="s">
-        <v>170</v>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K16" t="s">
         <v>292</v>
@@ -3330,8 +3354,9 @@
       <c r="I17">
         <v>1.63E-4</v>
       </c>
-      <c r="J17" t="s">
-        <v>170</v>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K17" t="s">
         <v>292</v>
@@ -3356,8 +3381,9 @@
       <c r="I18">
         <v>2.0699999999999999E-4</v>
       </c>
-      <c r="J18" t="s">
-        <v>170</v>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K18" t="s">
         <v>292</v>
@@ -3382,8 +3408,9 @@
       <c r="I19">
         <v>2.5799999999999998E-4</v>
       </c>
-      <c r="J19" t="s">
-        <v>170</v>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K19" t="s">
         <v>292</v>
@@ -3408,8 +3435,9 @@
       <c r="I20">
         <v>4.0400000000000001E-4</v>
       </c>
-      <c r="J20" t="s">
-        <v>170</v>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K20" t="s">
         <v>292</v>
@@ -3434,8 +3462,9 @@
       <c r="I21">
         <v>6.6399999999999999E-4</v>
       </c>
-      <c r="J21" t="s">
-        <v>170</v>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K21" t="s">
         <v>292</v>
@@ -3460,8 +3489,9 @@
       <c r="I22">
         <v>7.3499999999999998E-4</v>
       </c>
-      <c r="J22" t="s">
-        <v>170</v>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K22" t="s">
         <v>292</v>
@@ -3486,8 +3516,9 @@
       <c r="I23">
         <v>6.6399999999999999E-4</v>
       </c>
-      <c r="J23" t="s">
-        <v>170</v>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K23" t="s">
         <v>292</v>
@@ -3512,8 +3543,9 @@
       <c r="I24">
         <v>9.2800000000000001E-4</v>
       </c>
-      <c r="J24" t="s">
-        <v>170</v>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K24" t="s">
         <v>292</v>
@@ -3538,8 +3570,9 @@
       <c r="I25">
         <v>8.0500000000000005E-4</v>
       </c>
-      <c r="J25" t="s">
-        <v>170</v>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K25" t="s">
         <v>292</v>
@@ -3564,8 +3597,9 @@
       <c r="I26">
         <v>1.2099999999999999E-3</v>
       </c>
-      <c r="J26" t="s">
-        <v>170</v>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K26" t="s">
         <v>292</v>
@@ -3590,8 +3624,9 @@
       <c r="I27">
         <v>7.7200000000000001E-4</v>
       </c>
-      <c r="J27" t="s">
-        <v>170</v>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K27" t="s">
         <v>292</v>
@@ -3616,8 +3651,9 @@
       <c r="I28">
         <v>4.2900000000000002E-4</v>
       </c>
-      <c r="J28" t="s">
-        <v>170</v>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K28" t="s">
         <v>292</v>
@@ -3642,8 +3678,9 @@
       <c r="I29">
         <v>3.1399999999999999E-4</v>
       </c>
-      <c r="J29" t="s">
-        <v>170</v>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K29" t="s">
         <v>292</v>
@@ -3668,8 +3705,9 @@
       <c r="I30">
         <v>1.7699999999999999E-4</v>
       </c>
-      <c r="J30" t="s">
-        <v>170</v>
+      <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K30" t="s">
         <v>292</v>
@@ -3694,8 +3732,9 @@
       <c r="I31">
         <v>1.37E-4</v>
       </c>
-      <c r="J31" t="s">
-        <v>170</v>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K31" t="s">
         <v>292</v>
@@ -3720,8 +3759,9 @@
       <c r="I32">
         <v>1.16E-4</v>
       </c>
-      <c r="J32" t="s">
-        <v>170</v>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K32" t="s">
         <v>292</v>
@@ -3746,8 +3786,9 @@
       <c r="I33">
         <v>1.26E-4</v>
       </c>
-      <c r="J33" t="s">
-        <v>170</v>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K33" t="s">
         <v>292</v>
@@ -3772,8 +3813,9 @@
       <c r="I34">
         <v>2.23E-4</v>
       </c>
-      <c r="J34" t="s">
-        <v>170</v>
+      <c r="J34" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K34" t="s">
         <v>292</v>
@@ -3798,8 +3840,9 @@
       <c r="I35">
         <v>2.5799999999999998E-4</v>
       </c>
-      <c r="J35" t="s">
-        <v>170</v>
+      <c r="J35" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K35" t="s">
         <v>292</v>
@@ -3824,8 +3867,9 @@
       <c r="I36">
         <v>8.7482000000000004E-2</v>
       </c>
-      <c r="J36" t="s">
-        <v>170</v>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K36" t="s">
         <v>292</v>
@@ -3850,8 +3894,9 @@
       <c r="I37">
         <v>1.235E-2</v>
       </c>
-      <c r="J37" t="s">
-        <v>170</v>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K37" t="s">
         <v>292</v>
@@ -3876,8 +3921,9 @@
       <c r="I38">
         <v>1.2323000000000001E-2</v>
       </c>
-      <c r="J38" t="s">
-        <v>170</v>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K38" t="s">
         <v>292</v>
@@ -3902,8 +3948,9 @@
       <c r="I39">
         <v>1.2619E-2</v>
       </c>
-      <c r="J39" t="s">
-        <v>170</v>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K39" t="s">
         <v>292</v>
@@ -3928,8 +3975,9 @@
       <c r="I40">
         <v>7.4444999999999997E-2</v>
       </c>
-      <c r="J40" t="s">
-        <v>170</v>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K40" t="s">
         <v>292</v>
@@ -3954,8 +4002,9 @@
       <c r="I41">
         <v>1.7033E-2</v>
       </c>
-      <c r="J41" t="s">
-        <v>170</v>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K41" t="s">
         <v>292</v>
@@ -3980,8 +4029,9 @@
       <c r="I42">
         <v>1.6492E-2</v>
       </c>
-      <c r="J42" t="s">
-        <v>170</v>
+      <c r="J42" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K42" t="s">
         <v>292</v>
@@ -4006,8 +4056,9 @@
       <c r="I43">
         <v>9.2495999999999995E-2</v>
       </c>
-      <c r="J43" t="s">
-        <v>170</v>
+      <c r="J43" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K43" t="s">
         <v>292</v>
@@ -4032,8 +4083,9 @@
       <c r="I44">
         <v>1.02E-4</v>
       </c>
-      <c r="J44" t="s">
-        <v>170</v>
+      <c r="J44" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K44" t="s">
         <v>292</v>
@@ -4058,8 +4110,9 @@
       <c r="I45">
         <v>1.02E-4</v>
       </c>
-      <c r="J45" t="s">
-        <v>170</v>
+      <c r="J45" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K45" t="s">
         <v>292</v>
@@ -4084,8 +4137,9 @@
       <c r="I46">
         <v>1.02E-4</v>
       </c>
-      <c r="J46" t="s">
-        <v>170</v>
+      <c r="J46" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K46" t="s">
         <v>292</v>
@@ -4110,8 +4164,9 @@
       <c r="I47">
         <v>1.02E-4</v>
       </c>
-      <c r="J47" t="s">
-        <v>170</v>
+      <c r="J47" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K47" t="s">
         <v>292</v>
@@ -4136,8 +4191,9 @@
       <c r="I48">
         <v>1.02E-4</v>
       </c>
-      <c r="J48" t="s">
-        <v>170</v>
+      <c r="J48" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K48" t="s">
         <v>292</v>
@@ -4162,8 +4218,9 @@
       <c r="I49">
         <v>1.02E-4</v>
       </c>
-      <c r="J49" t="s">
-        <v>170</v>
+      <c r="J49" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K49" t="s">
         <v>292</v>
@@ -4188,8 +4245,9 @@
       <c r="I50">
         <v>1.02E-4</v>
       </c>
-      <c r="J50" t="s">
-        <v>170</v>
+      <c r="J50" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K50" t="s">
         <v>292</v>
@@ -4214,8 +4272,9 @@
       <c r="I51">
         <v>1.02E-4</v>
       </c>
-      <c r="J51" t="s">
-        <v>170</v>
+      <c r="J51" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K51" t="s">
         <v>292</v>
@@ -4240,8 +4299,9 @@
       <c r="I52">
         <v>1.02E-4</v>
       </c>
-      <c r="J52" t="s">
-        <v>170</v>
+      <c r="J52" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K52" t="s">
         <v>292</v>
@@ -4266,8 +4326,9 @@
       <c r="I53">
         <v>1.02E-4</v>
       </c>
-      <c r="J53" t="s">
-        <v>170</v>
+      <c r="J53" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K53" t="s">
         <v>292</v>
@@ -4292,8 +4353,9 @@
       <c r="I54">
         <v>1.02E-4</v>
       </c>
-      <c r="J54" t="s">
-        <v>170</v>
+      <c r="J54" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K54" t="s">
         <v>292</v>
@@ -4318,8 +4380,9 @@
       <c r="I55">
         <v>1.02E-4</v>
       </c>
-      <c r="J55" t="s">
-        <v>170</v>
+      <c r="J55" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K55" t="s">
         <v>292</v>
@@ -4344,8 +4407,9 @@
       <c r="I56">
         <v>1.02E-4</v>
       </c>
-      <c r="J56" t="s">
-        <v>170</v>
+      <c r="J56" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K56" t="s">
         <v>292</v>
@@ -4370,8 +4434,9 @@
       <c r="I57">
         <v>1.02E-4</v>
       </c>
-      <c r="J57" t="s">
-        <v>170</v>
+      <c r="J57" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K57" t="s">
         <v>292</v>
@@ -4396,8 +4461,9 @@
       <c r="I58">
         <v>1.02E-4</v>
       </c>
-      <c r="J58" t="s">
-        <v>170</v>
+      <c r="J58" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K58" t="s">
         <v>292</v>
@@ -4422,8 +4488,9 @@
       <c r="I59">
         <v>1.02E-4</v>
       </c>
-      <c r="J59" t="s">
-        <v>170</v>
+      <c r="J59" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K59" t="s">
         <v>292</v>
@@ -4448,8 +4515,9 @@
       <c r="I60">
         <v>1.02E-4</v>
       </c>
-      <c r="J60" t="s">
-        <v>170</v>
+      <c r="J60" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K60" t="s">
         <v>292</v>
@@ -4474,8 +4542,9 @@
       <c r="I61">
         <v>1.02E-4</v>
       </c>
-      <c r="J61" t="s">
-        <v>170</v>
+      <c r="J61" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K61" t="s">
         <v>292</v>
@@ -4500,8 +4569,9 @@
       <c r="I62">
         <v>1.02E-4</v>
       </c>
-      <c r="J62" t="s">
-        <v>170</v>
+      <c r="J62" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K62" t="s">
         <v>292</v>
@@ -4526,8 +4596,9 @@
       <c r="I63">
         <v>1.02E-4</v>
       </c>
-      <c r="J63" t="s">
-        <v>170</v>
+      <c r="J63" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K63" t="s">
         <v>292</v>
@@ -4552,8 +4623,9 @@
       <c r="I64">
         <v>1.02E-4</v>
       </c>
-      <c r="J64" t="s">
-        <v>170</v>
+      <c r="J64" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K64" t="s">
         <v>292</v>
@@ -4578,8 +4650,9 @@
       <c r="I65">
         <v>1.02E-4</v>
       </c>
-      <c r="J65" t="s">
-        <v>170</v>
+      <c r="J65" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K65" t="s">
         <v>292</v>
@@ -4604,8 +4677,9 @@
       <c r="I66">
         <v>1.02E-4</v>
       </c>
-      <c r="J66" t="s">
-        <v>170</v>
+      <c r="J66" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K66" t="s">
         <v>292</v>
@@ -4630,8 +4704,9 @@
       <c r="I67">
         <v>1.02E-4</v>
       </c>
-      <c r="J67" t="s">
-        <v>170</v>
+      <c r="J67" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K67" t="s">
         <v>292</v>
@@ -4656,8 +4731,9 @@
       <c r="I68">
         <v>1.02E-4</v>
       </c>
-      <c r="J68" t="s">
-        <v>170</v>
+      <c r="J68" t="str">
+        <f t="shared" si="0"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K68" t="s">
         <v>292</v>
@@ -4682,8 +4758,9 @@
       <c r="I69">
         <v>1.02E-4</v>
       </c>
-      <c r="J69" t="s">
-        <v>170</v>
+      <c r="J69" t="str">
+        <f t="shared" ref="J69:J123" si="1">K69</f>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K69" t="s">
         <v>292</v>
@@ -4708,8 +4785,9 @@
       <c r="I70">
         <v>1.02E-4</v>
       </c>
-      <c r="J70" t="s">
-        <v>170</v>
+      <c r="J70" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K70" t="s">
         <v>292</v>
@@ -4734,8 +4812,9 @@
       <c r="I71">
         <v>1.02E-4</v>
       </c>
-      <c r="J71" t="s">
-        <v>170</v>
+      <c r="J71" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K71" t="s">
         <v>292</v>
@@ -4760,8 +4839,9 @@
       <c r="I72">
         <v>1.02E-4</v>
       </c>
-      <c r="J72" t="s">
-        <v>170</v>
+      <c r="J72" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K72" t="s">
         <v>292</v>
@@ -4786,8 +4866,9 @@
       <c r="I73">
         <v>1.02E-4</v>
       </c>
-      <c r="J73" t="s">
-        <v>170</v>
+      <c r="J73" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K73" t="s">
         <v>292</v>
@@ -4812,8 +4893,9 @@
       <c r="I74">
         <v>1.02E-4</v>
       </c>
-      <c r="J74" t="s">
-        <v>170</v>
+      <c r="J74" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K74" t="s">
         <v>292</v>
@@ -4838,8 +4920,9 @@
       <c r="I75">
         <v>1.02E-4</v>
       </c>
-      <c r="J75" t="s">
-        <v>170</v>
+      <c r="J75" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K75" t="s">
         <v>292</v>
@@ -4864,8 +4947,9 @@
       <c r="I76">
         <v>1.02E-4</v>
       </c>
-      <c r="J76" t="s">
-        <v>170</v>
+      <c r="J76" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K76" t="s">
         <v>292</v>
@@ -4890,8 +4974,9 @@
       <c r="I77">
         <v>1.02E-4</v>
       </c>
-      <c r="J77" t="s">
-        <v>170</v>
+      <c r="J77" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K77" t="s">
         <v>292</v>
@@ -4916,8 +5001,9 @@
       <c r="I78">
         <v>1.02E-4</v>
       </c>
-      <c r="J78" t="s">
-        <v>170</v>
+      <c r="J78" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K78" t="s">
         <v>292</v>
@@ -4942,8 +5028,9 @@
       <c r="I79">
         <v>1.02E-4</v>
       </c>
-      <c r="J79" t="s">
-        <v>170</v>
+      <c r="J79" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K79" t="s">
         <v>292</v>
@@ -4968,8 +5055,9 @@
       <c r="I80">
         <v>1.02E-4</v>
       </c>
-      <c r="J80" t="s">
-        <v>170</v>
+      <c r="J80" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K80" t="s">
         <v>292</v>
@@ -4994,8 +5082,9 @@
       <c r="I81">
         <v>1.02E-4</v>
       </c>
-      <c r="J81" t="s">
-        <v>170</v>
+      <c r="J81" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K81" t="s">
         <v>292</v>
@@ -5020,8 +5109,9 @@
       <c r="I82">
         <v>1.02E-4</v>
       </c>
-      <c r="J82" t="s">
-        <v>170</v>
+      <c r="J82" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K82" t="s">
         <v>292</v>
@@ -5046,8 +5136,9 @@
       <c r="I83">
         <v>1.02E-4</v>
       </c>
-      <c r="J83" t="s">
-        <v>170</v>
+      <c r="J83" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K83" t="s">
         <v>292</v>
@@ -5072,8 +5163,9 @@
       <c r="I84">
         <v>1.02E-4</v>
       </c>
-      <c r="J84" t="s">
-        <v>170</v>
+      <c r="J84" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K84" t="s">
         <v>292</v>
@@ -5098,8 +5190,9 @@
       <c r="I85">
         <v>1.02E-4</v>
       </c>
-      <c r="J85" t="s">
-        <v>170</v>
+      <c r="J85" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K85" t="s">
         <v>292</v>
@@ -5124,8 +5217,9 @@
       <c r="I86">
         <v>1.02E-4</v>
       </c>
-      <c r="J86" t="s">
-        <v>170</v>
+      <c r="J86" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K86" t="s">
         <v>292</v>
@@ -5150,8 +5244,9 @@
       <c r="I87">
         <v>1.02E-4</v>
       </c>
-      <c r="J87" t="s">
-        <v>170</v>
+      <c r="J87" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K87" t="s">
         <v>292</v>
@@ -5176,8 +5271,9 @@
       <c r="I88">
         <v>1.02E-4</v>
       </c>
-      <c r="J88" t="s">
-        <v>170</v>
+      <c r="J88" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K88" t="s">
         <v>292</v>
@@ -5202,8 +5298,9 @@
       <c r="I89">
         <v>1.02E-4</v>
       </c>
-      <c r="J89" t="s">
-        <v>170</v>
+      <c r="J89" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K89" t="s">
         <v>292</v>
@@ -5228,8 +5325,9 @@
       <c r="I90">
         <v>1.02E-4</v>
       </c>
-      <c r="J90" t="s">
-        <v>170</v>
+      <c r="J90" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K90" t="s">
         <v>292</v>
@@ -5254,8 +5352,9 @@
       <c r="I91">
         <v>1.02E-4</v>
       </c>
-      <c r="J91" t="s">
-        <v>170</v>
+      <c r="J91" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K91" t="s">
         <v>292</v>
@@ -5280,8 +5379,9 @@
       <c r="I92">
         <v>4.4268000000000002E-2</v>
       </c>
-      <c r="J92" t="s">
-        <v>170</v>
+      <c r="J92" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K92" t="s">
         <v>292</v>
@@ -5306,8 +5406,9 @@
       <c r="I93">
         <v>6.3590000000000001E-3</v>
       </c>
-      <c r="J93" t="s">
-        <v>170</v>
+      <c r="J93" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K93" t="s">
         <v>292</v>
@@ -5332,8 +5433,9 @@
       <c r="I94">
         <v>6.3239999999999998E-3</v>
       </c>
-      <c r="J94" t="s">
-        <v>170</v>
+      <c r="J94" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K94" t="s">
         <v>292</v>
@@ -5358,8 +5460,9 @@
       <c r="I95">
         <v>6.3239999999999998E-3</v>
       </c>
-      <c r="J95" t="s">
-        <v>170</v>
+      <c r="J95" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K95" t="s">
         <v>292</v>
@@ -5384,8 +5487,9 @@
       <c r="I96">
         <v>3.3065999999999998E-2</v>
       </c>
-      <c r="J96" t="s">
-        <v>170</v>
+      <c r="J96" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K96" t="s">
         <v>292</v>
@@ -5410,8 +5514,9 @@
       <c r="I97">
         <v>7.2199999999999999E-3</v>
       </c>
-      <c r="J97" t="s">
-        <v>170</v>
+      <c r="J97" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K97" t="s">
         <v>292</v>
@@ -5436,8 +5541,9 @@
       <c r="I98">
         <v>7.0959999999999999E-3</v>
       </c>
-      <c r="J98" t="s">
-        <v>170</v>
+      <c r="J98" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K98" t="s">
         <v>292</v>
@@ -5462,8 +5568,9 @@
       <c r="I99">
         <v>4.4859000000000003E-2</v>
       </c>
-      <c r="J99" t="s">
-        <v>170</v>
+      <c r="J99" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K99" t="s">
         <v>292</v>
@@ -5488,8 +5595,9 @@
       <c r="I100">
         <v>4.6704999999999997E-2</v>
       </c>
-      <c r="J100" t="s">
-        <v>170</v>
+      <c r="J100" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K100" t="s">
         <v>292</v>
@@ -5514,8 +5622,9 @@
       <c r="I101">
         <v>6.5490000000000001E-3</v>
       </c>
-      <c r="J101" t="s">
-        <v>170</v>
+      <c r="J101" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K101" t="s">
         <v>292</v>
@@ -5540,8 +5649,9 @@
       <c r="I102">
         <v>6.5240000000000003E-3</v>
       </c>
-      <c r="J102" t="s">
-        <v>170</v>
+      <c r="J102" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K102" t="s">
         <v>292</v>
@@ -5566,8 +5676,9 @@
       <c r="I103">
         <v>6.5669999999999999E-3</v>
       </c>
-      <c r="J103" t="s">
-        <v>170</v>
+      <c r="J103" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K103" t="s">
         <v>292</v>
@@ -5592,8 +5703,9 @@
       <c r="I104">
         <v>3.6024E-2</v>
       </c>
-      <c r="J104" t="s">
-        <v>170</v>
+      <c r="J104" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K104" t="s">
         <v>292</v>
@@ -5618,8 +5730,9 @@
       <c r="I105">
         <v>7.6759999999999997E-3</v>
       </c>
-      <c r="J105" t="s">
-        <v>170</v>
+      <c r="J105" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K105" t="s">
         <v>292</v>
@@ -5644,8 +5757,9 @@
       <c r="I106">
         <v>8.1270000000000005E-3</v>
       </c>
-      <c r="J106" t="s">
-        <v>170</v>
+      <c r="J106" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K106" t="s">
         <v>292</v>
@@ -5670,8 +5784,9 @@
       <c r="I107">
         <v>4.8114999999999998E-2</v>
       </c>
-      <c r="J107" t="s">
-        <v>170</v>
+      <c r="J107" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K107" t="s">
         <v>292</v>
@@ -5696,8 +5811,9 @@
       <c r="I108">
         <v>2.3289000000000001E-2</v>
       </c>
-      <c r="J108" t="s">
-        <v>170</v>
+      <c r="J108" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K108" t="s">
         <v>292</v>
@@ -5722,8 +5838,9 @@
       <c r="I109">
         <v>3.3300000000000001E-3</v>
       </c>
-      <c r="J109" t="s">
-        <v>170</v>
+      <c r="J109" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K109" t="s">
         <v>292</v>
@@ -5748,8 +5865,9 @@
       <c r="I110">
         <v>3.2520000000000001E-3</v>
       </c>
-      <c r="J110" t="s">
-        <v>170</v>
+      <c r="J110" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K110" t="s">
         <v>292</v>
@@ -5774,8 +5892,9 @@
       <c r="I111">
         <v>3.5239999999999998E-3</v>
       </c>
-      <c r="J111" t="s">
-        <v>170</v>
+      <c r="J111" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K111" t="s">
         <v>292</v>
@@ -5800,8 +5919,9 @@
       <c r="I112">
         <v>2.8257999999999998E-2</v>
       </c>
-      <c r="J112" t="s">
-        <v>170</v>
+      <c r="J112" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K112" t="s">
         <v>292</v>
@@ -5826,8 +5946,9 @@
       <c r="I113">
         <v>5.0020000000000004E-3</v>
       </c>
-      <c r="J113" t="s">
-        <v>170</v>
+      <c r="J113" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K113" t="s">
         <v>292</v>
@@ -5852,8 +5973,9 @@
       <c r="I114">
         <v>4.6099999999999995E-3</v>
       </c>
-      <c r="J114" t="s">
-        <v>170</v>
+      <c r="J114" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K114" t="s">
         <v>292</v>
@@ -5878,8 +6000,9 @@
       <c r="I115">
         <v>2.3761999999999998E-2</v>
       </c>
-      <c r="J115" t="s">
-        <v>170</v>
+      <c r="J115" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K115" t="s">
         <v>292</v>
@@ -5904,8 +6027,9 @@
       <c r="I116">
         <v>2.2414E-2</v>
       </c>
-      <c r="J116" t="s">
-        <v>170</v>
+      <c r="J116" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K116" t="s">
         <v>292</v>
@@ -5930,8 +6054,9 @@
       <c r="I117">
         <v>3.176E-3</v>
       </c>
-      <c r="J117" t="s">
-        <v>170</v>
+      <c r="J117" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K117" t="s">
         <v>292</v>
@@ -5956,8 +6081,9 @@
       <c r="I118">
         <v>3.176E-3</v>
       </c>
-      <c r="J118" t="s">
-        <v>170</v>
+      <c r="J118" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K118" t="s">
         <v>292</v>
@@ -5982,8 +6108,9 @@
       <c r="I119">
         <v>3.1619999999999999E-3</v>
       </c>
-      <c r="J119" t="s">
-        <v>170</v>
+      <c r="J119" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K119" t="s">
         <v>292</v>
@@ -6008,8 +6135,9 @@
       <c r="I120">
         <v>1.5896E-2</v>
       </c>
-      <c r="J120" t="s">
-        <v>170</v>
+      <c r="J120" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K120" t="s">
         <v>292</v>
@@ -6034,8 +6162,9 @@
       <c r="I121">
         <v>3.3119999999999998E-3</v>
       </c>
-      <c r="J121" t="s">
-        <v>170</v>
+      <c r="J121" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K121" t="s">
         <v>292</v>
@@ -6060,8 +6189,9 @@
       <c r="I122">
         <v>3.2209999999999999E-3</v>
       </c>
-      <c r="J122" t="s">
-        <v>170</v>
+      <c r="J122" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K122" t="s">
         <v>292</v>
@@ -6086,8 +6216,9 @@
       <c r="I123">
         <v>2.2197999999999999E-2</v>
       </c>
-      <c r="J123" t="s">
-        <v>170</v>
+      <c r="J123" t="str">
+        <f t="shared" si="1"/>
+        <v>elc_won-CHE</v>
       </c>
       <c r="K123" t="s">
         <v>292</v>
@@ -6102,7 +6233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B35F46C-5F5C-47F6-BA1D-E82214B632D8}">
   <dimension ref="B2:O243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>

</xml_diff>